<commit_message>
visualized all 5 layers
</commit_message>
<xml_diff>
--- a/ArcTarget.xlsx
+++ b/ArcTarget.xlsx
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:M15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>